<commit_message>
curves : manual update of dt.init allowed
</commit_message>
<xml_diff>
--- a/input/curves/dsc.2.ir/xlsx/data.xlsx
+++ b/input/curves/dsc.2.ir/xlsx/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\data science\chemistry\kev\input\curves\dsc.2.ir\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74F0212-4CAC-4371-BCDF-4D1BE236544F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68AEAC1-D2A7-46E2-9F96-5FD65D120C55}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -369,7 +369,7 @@
   <dimension ref="A1:B210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B210"/>
+      <selection sqref="A1:B210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>